<commit_message>
Mise à jour JDT JLZ
Mise à jour du journal de travail
</commit_message>
<xml_diff>
--- a/DemoMotJDT-Lopezji.xlsx
+++ b/DemoMotJDT-Lopezji.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="71">
   <si>
     <t>Module :</t>
   </si>
@@ -258,6 +258,21 @@
   </si>
   <si>
     <t>Création du cahier des charges en vérifiant qu'il y ait assez de tâches pour mon collègue et moi. Nous avons fait des recherches pour savoir si l'utilisation d'un cms (typo3) est vraiment nécessaire ou productif pour notre projet. J'ai regardé deux vidéos, une qui résume ce qu'est typo 3 et une autre qui explique comment l'installer. Nous avons essayé chacun de nous de l'installer sur notre poste. une erreur est survenue lors de l'ouverture du fichier index.html présent dans le dossier de typo3. Elle indiquait qu'aucun fichier d'installation n'était présent. Il a fallu créer ce fichier en faisant une copie du fichier INSTALL déjà présent dans le dossier de typo3 et le renommer. Le navigateur propose alors une installation basique avec une interface assez complète. Une fois l'installation terminée, la page me propose de me connecter avec les identifiant d'administrateur entrés à l'installation mais au moment de la connexion, un chargement infini prend place et plus rien ne se passe. J'ai essayé de modifier les extensions utilisés dans le php.ini mais cela ne fonctionne toujours pas. Pas de solution pour le moment.</t>
+  </si>
+  <si>
+    <t>Daily scrum avec Fabien Pittier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mme Hardegger nous a aidé à comprendre comment fonctionne typo3 et l'installer </t>
+  </si>
+  <si>
+    <t>nous suivions un tutoriel qui nous montre les marches à suivre afin de mettre en place typo3 pour le site internet. Pendant la matinée nous avons appri à créer une page mère qui aura des sous pages, créer des templates afin de les charger pour une page ou plusieurs pages, modifier le nom et les propriétés d'une cellulle contenue dans un page (cellulle qui servira à insérer du contenu). Le tutoriel est effectué sur une ancienne version de typo3 ce qui cause du retard quand on cherche un menu précis ex: je cherchais comment modifier le template de la page mère mais dans l'ancienne version la page mère contient un template vide par défaut. Alors que je cherchais cette template, j'ai constaté qu'il fallait la créer car la nouvelle version n'en contient pas une de base. Un autre problème est survenu plus tard quand il fallait charger le template créé. Du code qui ne devait pas figurer dans le fichier main_1_column_with_menu.html a été généré et je ne connais malheureusement pas la raison de cette action. J'ai alors supprimé ce bout de code et cela fonctionne correctement. En lançant le site (index.php) il me ditait qu'il manquait une extension. Mon collègue et moi cherchions la solution pendant un bon moment jusqu'à ce que nous ayons décidé de demander de l'aide à Mme Hardegger. Elle nous a expliqué comment ajouter cette extension.</t>
+  </si>
+  <si>
+    <t>Création du mcd avec Jmerise (pas terminé)</t>
+  </si>
+  <si>
+    <t>J'ai continué à suivre le tutoriel qui m'a permis de comprendre l'utilité de faire plusiquers templates. J'ai aussi compris comment les attribuer à une page souhaitée.</t>
   </si>
 </sst>
 </file>
@@ -1347,6 +1362,12 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="16" fillId="6" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1355,12 +1376,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="6" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -3126,27 +3141,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId4" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId4" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>133350</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId4" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId4" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3176,27 +3191,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId8" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId8" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
+                <xdr:colOff>133350</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId8" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId8" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3234,470 +3249,470 @@
       <c r="C2" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="110" t="s">
+      <c r="D2" s="112" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
-      <c r="N2" s="111"/>
-      <c r="O2" s="111"/>
-      <c r="P2" s="111"/>
-      <c r="Q2" s="111"/>
-      <c r="R2" s="111"/>
-      <c r="S2" s="111"/>
-      <c r="T2" s="111"/>
-      <c r="U2" s="111"/>
-      <c r="V2" s="111"/>
-      <c r="W2" s="111"/>
-      <c r="X2" s="111"/>
-      <c r="Y2" s="111"/>
-      <c r="Z2" s="111"/>
-      <c r="AA2" s="111"/>
-      <c r="AB2" s="111"/>
-      <c r="AC2" s="111"/>
-      <c r="AD2" s="112"/>
-      <c r="AE2" s="110" t="s">
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="113"/>
+      <c r="O2" s="113"/>
+      <c r="P2" s="113"/>
+      <c r="Q2" s="113"/>
+      <c r="R2" s="113"/>
+      <c r="S2" s="113"/>
+      <c r="T2" s="113"/>
+      <c r="U2" s="113"/>
+      <c r="V2" s="113"/>
+      <c r="W2" s="113"/>
+      <c r="X2" s="113"/>
+      <c r="Y2" s="113"/>
+      <c r="Z2" s="113"/>
+      <c r="AA2" s="113"/>
+      <c r="AB2" s="113"/>
+      <c r="AC2" s="113"/>
+      <c r="AD2" s="114"/>
+      <c r="AE2" s="112" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="111"/>
-      <c r="AG2" s="111"/>
-      <c r="AH2" s="111"/>
-      <c r="AI2" s="111"/>
-      <c r="AJ2" s="111"/>
-      <c r="AK2" s="111"/>
-      <c r="AL2" s="111"/>
-      <c r="AM2" s="111"/>
-      <c r="AN2" s="111"/>
-      <c r="AO2" s="111"/>
-      <c r="AP2" s="111"/>
-      <c r="AQ2" s="111"/>
-      <c r="AR2" s="111"/>
-      <c r="AS2" s="111"/>
-      <c r="AT2" s="111"/>
-      <c r="AU2" s="111"/>
-      <c r="AV2" s="111"/>
-      <c r="AW2" s="111"/>
-      <c r="AX2" s="111"/>
-      <c r="AY2" s="111"/>
-      <c r="AZ2" s="111"/>
-      <c r="BA2" s="111"/>
-      <c r="BB2" s="111"/>
-      <c r="BC2" s="111"/>
-      <c r="BD2" s="111"/>
-      <c r="BE2" s="112"/>
-      <c r="BF2" s="110" t="s">
+      <c r="AF2" s="113"/>
+      <c r="AG2" s="113"/>
+      <c r="AH2" s="113"/>
+      <c r="AI2" s="113"/>
+      <c r="AJ2" s="113"/>
+      <c r="AK2" s="113"/>
+      <c r="AL2" s="113"/>
+      <c r="AM2" s="113"/>
+      <c r="AN2" s="113"/>
+      <c r="AO2" s="113"/>
+      <c r="AP2" s="113"/>
+      <c r="AQ2" s="113"/>
+      <c r="AR2" s="113"/>
+      <c r="AS2" s="113"/>
+      <c r="AT2" s="113"/>
+      <c r="AU2" s="113"/>
+      <c r="AV2" s="113"/>
+      <c r="AW2" s="113"/>
+      <c r="AX2" s="113"/>
+      <c r="AY2" s="113"/>
+      <c r="AZ2" s="113"/>
+      <c r="BA2" s="113"/>
+      <c r="BB2" s="113"/>
+      <c r="BC2" s="113"/>
+      <c r="BD2" s="113"/>
+      <c r="BE2" s="114"/>
+      <c r="BF2" s="112" t="s">
         <v>30</v>
       </c>
-      <c r="BG2" s="111"/>
-      <c r="BH2" s="111"/>
-      <c r="BI2" s="111"/>
-      <c r="BJ2" s="111"/>
-      <c r="BK2" s="111"/>
-      <c r="BL2" s="111"/>
-      <c r="BM2" s="111"/>
-      <c r="BN2" s="111"/>
-      <c r="BO2" s="111"/>
-      <c r="BP2" s="111"/>
-      <c r="BQ2" s="111"/>
-      <c r="BR2" s="111"/>
-      <c r="BS2" s="111"/>
-      <c r="BT2" s="111"/>
-      <c r="BU2" s="111"/>
-      <c r="BV2" s="111"/>
-      <c r="BW2" s="111"/>
-      <c r="BX2" s="111"/>
-      <c r="BY2" s="111"/>
-      <c r="BZ2" s="111"/>
-      <c r="CA2" s="111"/>
-      <c r="CB2" s="111"/>
-      <c r="CC2" s="111"/>
-      <c r="CD2" s="111"/>
-      <c r="CE2" s="111"/>
-      <c r="CF2" s="112"/>
-      <c r="CG2" s="110" t="s">
+      <c r="BG2" s="113"/>
+      <c r="BH2" s="113"/>
+      <c r="BI2" s="113"/>
+      <c r="BJ2" s="113"/>
+      <c r="BK2" s="113"/>
+      <c r="BL2" s="113"/>
+      <c r="BM2" s="113"/>
+      <c r="BN2" s="113"/>
+      <c r="BO2" s="113"/>
+      <c r="BP2" s="113"/>
+      <c r="BQ2" s="113"/>
+      <c r="BR2" s="113"/>
+      <c r="BS2" s="113"/>
+      <c r="BT2" s="113"/>
+      <c r="BU2" s="113"/>
+      <c r="BV2" s="113"/>
+      <c r="BW2" s="113"/>
+      <c r="BX2" s="113"/>
+      <c r="BY2" s="113"/>
+      <c r="BZ2" s="113"/>
+      <c r="CA2" s="113"/>
+      <c r="CB2" s="113"/>
+      <c r="CC2" s="113"/>
+      <c r="CD2" s="113"/>
+      <c r="CE2" s="113"/>
+      <c r="CF2" s="114"/>
+      <c r="CG2" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="CH2" s="111"/>
-      <c r="CI2" s="111"/>
-      <c r="CJ2" s="111"/>
-      <c r="CK2" s="111"/>
-      <c r="CL2" s="111"/>
-      <c r="CM2" s="111"/>
-      <c r="CN2" s="111"/>
-      <c r="CO2" s="111"/>
-      <c r="CP2" s="111"/>
-      <c r="CQ2" s="111"/>
-      <c r="CR2" s="111"/>
-      <c r="CS2" s="111"/>
-      <c r="CT2" s="111"/>
-      <c r="CU2" s="111"/>
-      <c r="CV2" s="111"/>
-      <c r="CW2" s="111"/>
-      <c r="CX2" s="111"/>
-      <c r="CY2" s="111"/>
-      <c r="CZ2" s="111"/>
-      <c r="DA2" s="111"/>
-      <c r="DB2" s="111"/>
-      <c r="DC2" s="111"/>
-      <c r="DD2" s="111"/>
-      <c r="DE2" s="111"/>
-      <c r="DF2" s="111"/>
-      <c r="DG2" s="112"/>
-      <c r="DH2" s="110" t="s">
+      <c r="CH2" s="113"/>
+      <c r="CI2" s="113"/>
+      <c r="CJ2" s="113"/>
+      <c r="CK2" s="113"/>
+      <c r="CL2" s="113"/>
+      <c r="CM2" s="113"/>
+      <c r="CN2" s="113"/>
+      <c r="CO2" s="113"/>
+      <c r="CP2" s="113"/>
+      <c r="CQ2" s="113"/>
+      <c r="CR2" s="113"/>
+      <c r="CS2" s="113"/>
+      <c r="CT2" s="113"/>
+      <c r="CU2" s="113"/>
+      <c r="CV2" s="113"/>
+      <c r="CW2" s="113"/>
+      <c r="CX2" s="113"/>
+      <c r="CY2" s="113"/>
+      <c r="CZ2" s="113"/>
+      <c r="DA2" s="113"/>
+      <c r="DB2" s="113"/>
+      <c r="DC2" s="113"/>
+      <c r="DD2" s="113"/>
+      <c r="DE2" s="113"/>
+      <c r="DF2" s="113"/>
+      <c r="DG2" s="114"/>
+      <c r="DH2" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="DI2" s="111"/>
-      <c r="DJ2" s="111"/>
-      <c r="DK2" s="111"/>
-      <c r="DL2" s="111"/>
-      <c r="DM2" s="111"/>
-      <c r="DN2" s="111"/>
-      <c r="DO2" s="111"/>
-      <c r="DP2" s="111"/>
-      <c r="DQ2" s="111"/>
-      <c r="DR2" s="111"/>
-      <c r="DS2" s="111"/>
-      <c r="DT2" s="111"/>
-      <c r="DU2" s="111"/>
-      <c r="DV2" s="111"/>
-      <c r="DW2" s="111"/>
-      <c r="DX2" s="111"/>
-      <c r="DY2" s="111"/>
-      <c r="DZ2" s="111"/>
-      <c r="EA2" s="111"/>
-      <c r="EB2" s="111"/>
-      <c r="EC2" s="111"/>
-      <c r="ED2" s="111"/>
-      <c r="EE2" s="111"/>
-      <c r="EF2" s="111"/>
-      <c r="EG2" s="111"/>
-      <c r="EH2" s="112"/>
-      <c r="EI2" s="110" t="s">
+      <c r="DI2" s="113"/>
+      <c r="DJ2" s="113"/>
+      <c r="DK2" s="113"/>
+      <c r="DL2" s="113"/>
+      <c r="DM2" s="113"/>
+      <c r="DN2" s="113"/>
+      <c r="DO2" s="113"/>
+      <c r="DP2" s="113"/>
+      <c r="DQ2" s="113"/>
+      <c r="DR2" s="113"/>
+      <c r="DS2" s="113"/>
+      <c r="DT2" s="113"/>
+      <c r="DU2" s="113"/>
+      <c r="DV2" s="113"/>
+      <c r="DW2" s="113"/>
+      <c r="DX2" s="113"/>
+      <c r="DY2" s="113"/>
+      <c r="DZ2" s="113"/>
+      <c r="EA2" s="113"/>
+      <c r="EB2" s="113"/>
+      <c r="EC2" s="113"/>
+      <c r="ED2" s="113"/>
+      <c r="EE2" s="113"/>
+      <c r="EF2" s="113"/>
+      <c r="EG2" s="113"/>
+      <c r="EH2" s="114"/>
+      <c r="EI2" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="EJ2" s="111"/>
-      <c r="EK2" s="111"/>
-      <c r="EL2" s="111"/>
-      <c r="EM2" s="111"/>
-      <c r="EN2" s="111"/>
-      <c r="EO2" s="111"/>
-      <c r="EP2" s="111"/>
-      <c r="EQ2" s="111"/>
-      <c r="ER2" s="111"/>
-      <c r="ES2" s="111"/>
-      <c r="ET2" s="111"/>
-      <c r="EU2" s="111"/>
-      <c r="EV2" s="111"/>
-      <c r="EW2" s="111"/>
-      <c r="EX2" s="111"/>
-      <c r="EY2" s="111"/>
-      <c r="EZ2" s="111"/>
-      <c r="FA2" s="111"/>
-      <c r="FB2" s="111"/>
-      <c r="FC2" s="111"/>
-      <c r="FD2" s="111"/>
-      <c r="FE2" s="111"/>
-      <c r="FF2" s="111"/>
-      <c r="FG2" s="111"/>
-      <c r="FH2" s="111"/>
-      <c r="FI2" s="112"/>
-      <c r="FJ2" s="110" t="s">
+      <c r="EJ2" s="113"/>
+      <c r="EK2" s="113"/>
+      <c r="EL2" s="113"/>
+      <c r="EM2" s="113"/>
+      <c r="EN2" s="113"/>
+      <c r="EO2" s="113"/>
+      <c r="EP2" s="113"/>
+      <c r="EQ2" s="113"/>
+      <c r="ER2" s="113"/>
+      <c r="ES2" s="113"/>
+      <c r="ET2" s="113"/>
+      <c r="EU2" s="113"/>
+      <c r="EV2" s="113"/>
+      <c r="EW2" s="113"/>
+      <c r="EX2" s="113"/>
+      <c r="EY2" s="113"/>
+      <c r="EZ2" s="113"/>
+      <c r="FA2" s="113"/>
+      <c r="FB2" s="113"/>
+      <c r="FC2" s="113"/>
+      <c r="FD2" s="113"/>
+      <c r="FE2" s="113"/>
+      <c r="FF2" s="113"/>
+      <c r="FG2" s="113"/>
+      <c r="FH2" s="113"/>
+      <c r="FI2" s="114"/>
+      <c r="FJ2" s="112" t="s">
         <v>34</v>
       </c>
-      <c r="FK2" s="111"/>
-      <c r="FL2" s="111"/>
-      <c r="FM2" s="111"/>
-      <c r="FN2" s="111"/>
-      <c r="FO2" s="111"/>
-      <c r="FP2" s="111"/>
-      <c r="FQ2" s="111"/>
-      <c r="FR2" s="111"/>
-      <c r="FS2" s="111"/>
-      <c r="FT2" s="111"/>
-      <c r="FU2" s="111"/>
-      <c r="FV2" s="111"/>
-      <c r="FW2" s="111"/>
-      <c r="FX2" s="111"/>
-      <c r="FY2" s="111"/>
-      <c r="FZ2" s="111"/>
-      <c r="GA2" s="111"/>
-      <c r="GB2" s="111"/>
-      <c r="GC2" s="111"/>
-      <c r="GD2" s="111"/>
-      <c r="GE2" s="111"/>
-      <c r="GF2" s="111"/>
-      <c r="GG2" s="111"/>
-      <c r="GH2" s="111"/>
-      <c r="GI2" s="111"/>
-      <c r="GJ2" s="112"/>
-      <c r="GK2" s="110" t="s">
+      <c r="FK2" s="113"/>
+      <c r="FL2" s="113"/>
+      <c r="FM2" s="113"/>
+      <c r="FN2" s="113"/>
+      <c r="FO2" s="113"/>
+      <c r="FP2" s="113"/>
+      <c r="FQ2" s="113"/>
+      <c r="FR2" s="113"/>
+      <c r="FS2" s="113"/>
+      <c r="FT2" s="113"/>
+      <c r="FU2" s="113"/>
+      <c r="FV2" s="113"/>
+      <c r="FW2" s="113"/>
+      <c r="FX2" s="113"/>
+      <c r="FY2" s="113"/>
+      <c r="FZ2" s="113"/>
+      <c r="GA2" s="113"/>
+      <c r="GB2" s="113"/>
+      <c r="GC2" s="113"/>
+      <c r="GD2" s="113"/>
+      <c r="GE2" s="113"/>
+      <c r="GF2" s="113"/>
+      <c r="GG2" s="113"/>
+      <c r="GH2" s="113"/>
+      <c r="GI2" s="113"/>
+      <c r="GJ2" s="114"/>
+      <c r="GK2" s="112" t="s">
         <v>35</v>
       </c>
-      <c r="GL2" s="111"/>
-      <c r="GM2" s="111"/>
-      <c r="GN2" s="111"/>
-      <c r="GO2" s="111"/>
-      <c r="GP2" s="111"/>
-      <c r="GQ2" s="111"/>
-      <c r="GR2" s="111"/>
-      <c r="GS2" s="111"/>
-      <c r="GT2" s="111"/>
-      <c r="GU2" s="111"/>
-      <c r="GV2" s="111"/>
-      <c r="GW2" s="111"/>
-      <c r="GX2" s="111"/>
-      <c r="GY2" s="111"/>
-      <c r="GZ2" s="111"/>
-      <c r="HA2" s="111"/>
-      <c r="HB2" s="111"/>
-      <c r="HC2" s="111"/>
-      <c r="HD2" s="111"/>
-      <c r="HE2" s="111"/>
-      <c r="HF2" s="111"/>
-      <c r="HG2" s="111"/>
-      <c r="HH2" s="111"/>
-      <c r="HI2" s="111"/>
-      <c r="HJ2" s="111"/>
-      <c r="HK2" s="112"/>
-      <c r="HL2" s="110" t="s">
+      <c r="GL2" s="113"/>
+      <c r="GM2" s="113"/>
+      <c r="GN2" s="113"/>
+      <c r="GO2" s="113"/>
+      <c r="GP2" s="113"/>
+      <c r="GQ2" s="113"/>
+      <c r="GR2" s="113"/>
+      <c r="GS2" s="113"/>
+      <c r="GT2" s="113"/>
+      <c r="GU2" s="113"/>
+      <c r="GV2" s="113"/>
+      <c r="GW2" s="113"/>
+      <c r="GX2" s="113"/>
+      <c r="GY2" s="113"/>
+      <c r="GZ2" s="113"/>
+      <c r="HA2" s="113"/>
+      <c r="HB2" s="113"/>
+      <c r="HC2" s="113"/>
+      <c r="HD2" s="113"/>
+      <c r="HE2" s="113"/>
+      <c r="HF2" s="113"/>
+      <c r="HG2" s="113"/>
+      <c r="HH2" s="113"/>
+      <c r="HI2" s="113"/>
+      <c r="HJ2" s="113"/>
+      <c r="HK2" s="114"/>
+      <c r="HL2" s="112" t="s">
         <v>36</v>
       </c>
-      <c r="HM2" s="111"/>
-      <c r="HN2" s="111"/>
-      <c r="HO2" s="111"/>
-      <c r="HP2" s="111"/>
-      <c r="HQ2" s="111"/>
-      <c r="HR2" s="111"/>
-      <c r="HS2" s="111"/>
-      <c r="HT2" s="111"/>
-      <c r="HU2" s="111"/>
-      <c r="HV2" s="111"/>
-      <c r="HW2" s="111"/>
-      <c r="HX2" s="111"/>
-      <c r="HY2" s="111"/>
-      <c r="HZ2" s="111"/>
-      <c r="IA2" s="111"/>
-      <c r="IB2" s="111"/>
-      <c r="IC2" s="111"/>
-      <c r="ID2" s="111"/>
-      <c r="IE2" s="111"/>
-      <c r="IF2" s="111"/>
-      <c r="IG2" s="111"/>
-      <c r="IH2" s="111"/>
-      <c r="II2" s="111"/>
-      <c r="IJ2" s="111"/>
-      <c r="IK2" s="111"/>
-      <c r="IL2" s="112"/>
-      <c r="IM2" s="110" t="s">
+      <c r="HM2" s="113"/>
+      <c r="HN2" s="113"/>
+      <c r="HO2" s="113"/>
+      <c r="HP2" s="113"/>
+      <c r="HQ2" s="113"/>
+      <c r="HR2" s="113"/>
+      <c r="HS2" s="113"/>
+      <c r="HT2" s="113"/>
+      <c r="HU2" s="113"/>
+      <c r="HV2" s="113"/>
+      <c r="HW2" s="113"/>
+      <c r="HX2" s="113"/>
+      <c r="HY2" s="113"/>
+      <c r="HZ2" s="113"/>
+      <c r="IA2" s="113"/>
+      <c r="IB2" s="113"/>
+      <c r="IC2" s="113"/>
+      <c r="ID2" s="113"/>
+      <c r="IE2" s="113"/>
+      <c r="IF2" s="113"/>
+      <c r="IG2" s="113"/>
+      <c r="IH2" s="113"/>
+      <c r="II2" s="113"/>
+      <c r="IJ2" s="113"/>
+      <c r="IK2" s="113"/>
+      <c r="IL2" s="114"/>
+      <c r="IM2" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="IN2" s="111"/>
-      <c r="IO2" s="111"/>
-      <c r="IP2" s="111"/>
-      <c r="IQ2" s="111"/>
-      <c r="IR2" s="111"/>
-      <c r="IS2" s="111"/>
-      <c r="IT2" s="111"/>
-      <c r="IU2" s="111"/>
-      <c r="IV2" s="111"/>
-      <c r="IW2" s="111"/>
-      <c r="IX2" s="111"/>
-      <c r="IY2" s="111"/>
-      <c r="IZ2" s="111"/>
-      <c r="JA2" s="111"/>
-      <c r="JB2" s="111"/>
-      <c r="JC2" s="111"/>
-      <c r="JD2" s="111"/>
-      <c r="JE2" s="111"/>
-      <c r="JF2" s="111"/>
-      <c r="JG2" s="111"/>
-      <c r="JH2" s="111"/>
-      <c r="JI2" s="111"/>
-      <c r="JJ2" s="111"/>
-      <c r="JK2" s="111"/>
-      <c r="JL2" s="111"/>
-      <c r="JM2" s="112"/>
-      <c r="JN2" s="110" t="s">
+      <c r="IN2" s="113"/>
+      <c r="IO2" s="113"/>
+      <c r="IP2" s="113"/>
+      <c r="IQ2" s="113"/>
+      <c r="IR2" s="113"/>
+      <c r="IS2" s="113"/>
+      <c r="IT2" s="113"/>
+      <c r="IU2" s="113"/>
+      <c r="IV2" s="113"/>
+      <c r="IW2" s="113"/>
+      <c r="IX2" s="113"/>
+      <c r="IY2" s="113"/>
+      <c r="IZ2" s="113"/>
+      <c r="JA2" s="113"/>
+      <c r="JB2" s="113"/>
+      <c r="JC2" s="113"/>
+      <c r="JD2" s="113"/>
+      <c r="JE2" s="113"/>
+      <c r="JF2" s="113"/>
+      <c r="JG2" s="113"/>
+      <c r="JH2" s="113"/>
+      <c r="JI2" s="113"/>
+      <c r="JJ2" s="113"/>
+      <c r="JK2" s="113"/>
+      <c r="JL2" s="113"/>
+      <c r="JM2" s="114"/>
+      <c r="JN2" s="112" t="s">
         <v>38</v>
       </c>
-      <c r="JO2" s="111"/>
-      <c r="JP2" s="111"/>
-      <c r="JQ2" s="111"/>
-      <c r="JR2" s="111"/>
-      <c r="JS2" s="111"/>
-      <c r="JT2" s="111"/>
-      <c r="JU2" s="111"/>
-      <c r="JV2" s="111"/>
-      <c r="JW2" s="111"/>
-      <c r="JX2" s="111"/>
-      <c r="JY2" s="111"/>
-      <c r="JZ2" s="111"/>
-      <c r="KA2" s="111"/>
-      <c r="KB2" s="111"/>
-      <c r="KC2" s="111"/>
-      <c r="KD2" s="111"/>
-      <c r="KE2" s="111"/>
-      <c r="KF2" s="111"/>
-      <c r="KG2" s="111"/>
-      <c r="KH2" s="111"/>
-      <c r="KI2" s="111"/>
-      <c r="KJ2" s="111"/>
-      <c r="KK2" s="111"/>
-      <c r="KL2" s="111"/>
-      <c r="KM2" s="111"/>
-      <c r="KN2" s="112"/>
-      <c r="KO2" s="110" t="s">
+      <c r="JO2" s="113"/>
+      <c r="JP2" s="113"/>
+      <c r="JQ2" s="113"/>
+      <c r="JR2" s="113"/>
+      <c r="JS2" s="113"/>
+      <c r="JT2" s="113"/>
+      <c r="JU2" s="113"/>
+      <c r="JV2" s="113"/>
+      <c r="JW2" s="113"/>
+      <c r="JX2" s="113"/>
+      <c r="JY2" s="113"/>
+      <c r="JZ2" s="113"/>
+      <c r="KA2" s="113"/>
+      <c r="KB2" s="113"/>
+      <c r="KC2" s="113"/>
+      <c r="KD2" s="113"/>
+      <c r="KE2" s="113"/>
+      <c r="KF2" s="113"/>
+      <c r="KG2" s="113"/>
+      <c r="KH2" s="113"/>
+      <c r="KI2" s="113"/>
+      <c r="KJ2" s="113"/>
+      <c r="KK2" s="113"/>
+      <c r="KL2" s="113"/>
+      <c r="KM2" s="113"/>
+      <c r="KN2" s="114"/>
+      <c r="KO2" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="KP2" s="111"/>
-      <c r="KQ2" s="111"/>
-      <c r="KR2" s="111"/>
-      <c r="KS2" s="111"/>
-      <c r="KT2" s="111"/>
-      <c r="KU2" s="111"/>
-      <c r="KV2" s="111"/>
-      <c r="KW2" s="111"/>
-      <c r="KX2" s="111"/>
-      <c r="KY2" s="111"/>
-      <c r="KZ2" s="111"/>
-      <c r="LA2" s="111"/>
-      <c r="LB2" s="111"/>
-      <c r="LC2" s="111"/>
-      <c r="LD2" s="111"/>
-      <c r="LE2" s="111"/>
-      <c r="LF2" s="111"/>
-      <c r="LG2" s="111"/>
-      <c r="LH2" s="111"/>
-      <c r="LI2" s="111"/>
-      <c r="LJ2" s="111"/>
-      <c r="LK2" s="111"/>
-      <c r="LL2" s="111"/>
-      <c r="LM2" s="111"/>
-      <c r="LN2" s="111"/>
-      <c r="LO2" s="112"/>
-      <c r="LP2" s="110" t="s">
+      <c r="KP2" s="113"/>
+      <c r="KQ2" s="113"/>
+      <c r="KR2" s="113"/>
+      <c r="KS2" s="113"/>
+      <c r="KT2" s="113"/>
+      <c r="KU2" s="113"/>
+      <c r="KV2" s="113"/>
+      <c r="KW2" s="113"/>
+      <c r="KX2" s="113"/>
+      <c r="KY2" s="113"/>
+      <c r="KZ2" s="113"/>
+      <c r="LA2" s="113"/>
+      <c r="LB2" s="113"/>
+      <c r="LC2" s="113"/>
+      <c r="LD2" s="113"/>
+      <c r="LE2" s="113"/>
+      <c r="LF2" s="113"/>
+      <c r="LG2" s="113"/>
+      <c r="LH2" s="113"/>
+      <c r="LI2" s="113"/>
+      <c r="LJ2" s="113"/>
+      <c r="LK2" s="113"/>
+      <c r="LL2" s="113"/>
+      <c r="LM2" s="113"/>
+      <c r="LN2" s="113"/>
+      <c r="LO2" s="114"/>
+      <c r="LP2" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="LQ2" s="111"/>
-      <c r="LR2" s="111"/>
-      <c r="LS2" s="111"/>
-      <c r="LT2" s="111"/>
-      <c r="LU2" s="111"/>
-      <c r="LV2" s="111"/>
-      <c r="LW2" s="111"/>
-      <c r="LX2" s="111"/>
-      <c r="LY2" s="111"/>
-      <c r="LZ2" s="111"/>
-      <c r="MA2" s="111"/>
-      <c r="MB2" s="111"/>
-      <c r="MC2" s="111"/>
-      <c r="MD2" s="111"/>
-      <c r="ME2" s="111"/>
-      <c r="MF2" s="111"/>
-      <c r="MG2" s="111"/>
-      <c r="MH2" s="111"/>
-      <c r="MI2" s="111"/>
-      <c r="MJ2" s="111"/>
-      <c r="MK2" s="111"/>
-      <c r="ML2" s="111"/>
-      <c r="MM2" s="111"/>
-      <c r="MN2" s="111"/>
-      <c r="MO2" s="111"/>
-      <c r="MP2" s="112"/>
-      <c r="MQ2" s="110" t="s">
+      <c r="LQ2" s="113"/>
+      <c r="LR2" s="113"/>
+      <c r="LS2" s="113"/>
+      <c r="LT2" s="113"/>
+      <c r="LU2" s="113"/>
+      <c r="LV2" s="113"/>
+      <c r="LW2" s="113"/>
+      <c r="LX2" s="113"/>
+      <c r="LY2" s="113"/>
+      <c r="LZ2" s="113"/>
+      <c r="MA2" s="113"/>
+      <c r="MB2" s="113"/>
+      <c r="MC2" s="113"/>
+      <c r="MD2" s="113"/>
+      <c r="ME2" s="113"/>
+      <c r="MF2" s="113"/>
+      <c r="MG2" s="113"/>
+      <c r="MH2" s="113"/>
+      <c r="MI2" s="113"/>
+      <c r="MJ2" s="113"/>
+      <c r="MK2" s="113"/>
+      <c r="ML2" s="113"/>
+      <c r="MM2" s="113"/>
+      <c r="MN2" s="113"/>
+      <c r="MO2" s="113"/>
+      <c r="MP2" s="114"/>
+      <c r="MQ2" s="112" t="s">
         <v>41</v>
       </c>
-      <c r="MR2" s="111"/>
-      <c r="MS2" s="111"/>
-      <c r="MT2" s="111"/>
-      <c r="MU2" s="111"/>
-      <c r="MV2" s="111"/>
-      <c r="MW2" s="111"/>
-      <c r="MX2" s="111"/>
-      <c r="MY2" s="111"/>
-      <c r="MZ2" s="111"/>
-      <c r="NA2" s="111"/>
-      <c r="NB2" s="111"/>
-      <c r="NC2" s="111"/>
-      <c r="ND2" s="111"/>
-      <c r="NE2" s="111"/>
-      <c r="NF2" s="111"/>
-      <c r="NG2" s="111"/>
-      <c r="NH2" s="111"/>
-      <c r="NI2" s="111"/>
-      <c r="NJ2" s="111"/>
-      <c r="NK2" s="111"/>
-      <c r="NL2" s="111"/>
-      <c r="NM2" s="111"/>
-      <c r="NN2" s="111"/>
-      <c r="NO2" s="111"/>
-      <c r="NP2" s="111"/>
-      <c r="NQ2" s="112"/>
-      <c r="NR2" s="110" t="s">
+      <c r="MR2" s="113"/>
+      <c r="MS2" s="113"/>
+      <c r="MT2" s="113"/>
+      <c r="MU2" s="113"/>
+      <c r="MV2" s="113"/>
+      <c r="MW2" s="113"/>
+      <c r="MX2" s="113"/>
+      <c r="MY2" s="113"/>
+      <c r="MZ2" s="113"/>
+      <c r="NA2" s="113"/>
+      <c r="NB2" s="113"/>
+      <c r="NC2" s="113"/>
+      <c r="ND2" s="113"/>
+      <c r="NE2" s="113"/>
+      <c r="NF2" s="113"/>
+      <c r="NG2" s="113"/>
+      <c r="NH2" s="113"/>
+      <c r="NI2" s="113"/>
+      <c r="NJ2" s="113"/>
+      <c r="NK2" s="113"/>
+      <c r="NL2" s="113"/>
+      <c r="NM2" s="113"/>
+      <c r="NN2" s="113"/>
+      <c r="NO2" s="113"/>
+      <c r="NP2" s="113"/>
+      <c r="NQ2" s="114"/>
+      <c r="NR2" s="112" t="s">
         <v>42</v>
       </c>
-      <c r="NS2" s="111"/>
-      <c r="NT2" s="111"/>
-      <c r="NU2" s="111"/>
-      <c r="NV2" s="111"/>
-      <c r="NW2" s="111"/>
-      <c r="NX2" s="111"/>
-      <c r="NY2" s="111"/>
-      <c r="NZ2" s="111"/>
-      <c r="OA2" s="111"/>
-      <c r="OB2" s="111"/>
-      <c r="OC2" s="111"/>
-      <c r="OD2" s="111"/>
-      <c r="OE2" s="111"/>
-      <c r="OF2" s="111"/>
-      <c r="OG2" s="111"/>
-      <c r="OH2" s="111"/>
-      <c r="OI2" s="111"/>
-      <c r="OJ2" s="111"/>
-      <c r="OK2" s="111"/>
-      <c r="OL2" s="111"/>
-      <c r="OM2" s="111"/>
-      <c r="ON2" s="111"/>
-      <c r="OO2" s="111"/>
-      <c r="OP2" s="111"/>
-      <c r="OQ2" s="111"/>
-      <c r="OR2" s="112"/>
-      <c r="OS2" s="110" t="s">
+      <c r="NS2" s="113"/>
+      <c r="NT2" s="113"/>
+      <c r="NU2" s="113"/>
+      <c r="NV2" s="113"/>
+      <c r="NW2" s="113"/>
+      <c r="NX2" s="113"/>
+      <c r="NY2" s="113"/>
+      <c r="NZ2" s="113"/>
+      <c r="OA2" s="113"/>
+      <c r="OB2" s="113"/>
+      <c r="OC2" s="113"/>
+      <c r="OD2" s="113"/>
+      <c r="OE2" s="113"/>
+      <c r="OF2" s="113"/>
+      <c r="OG2" s="113"/>
+      <c r="OH2" s="113"/>
+      <c r="OI2" s="113"/>
+      <c r="OJ2" s="113"/>
+      <c r="OK2" s="113"/>
+      <c r="OL2" s="113"/>
+      <c r="OM2" s="113"/>
+      <c r="ON2" s="113"/>
+      <c r="OO2" s="113"/>
+      <c r="OP2" s="113"/>
+      <c r="OQ2" s="113"/>
+      <c r="OR2" s="114"/>
+      <c r="OS2" s="112" t="s">
         <v>43</v>
       </c>
-      <c r="OT2" s="111"/>
-      <c r="OU2" s="111"/>
-      <c r="OV2" s="111"/>
-      <c r="OW2" s="111"/>
-      <c r="OX2" s="111"/>
-      <c r="OY2" s="111"/>
-      <c r="OZ2" s="111"/>
-      <c r="PA2" s="111"/>
-      <c r="PB2" s="111"/>
-      <c r="PC2" s="111"/>
-      <c r="PD2" s="111"/>
-      <c r="PE2" s="111"/>
-      <c r="PF2" s="111"/>
-      <c r="PG2" s="111"/>
-      <c r="PH2" s="111"/>
-      <c r="PI2" s="111"/>
-      <c r="PJ2" s="111"/>
-      <c r="PK2" s="111"/>
-      <c r="PL2" s="111"/>
-      <c r="PM2" s="111"/>
-      <c r="PN2" s="111"/>
-      <c r="PO2" s="111"/>
-      <c r="PP2" s="111"/>
-      <c r="PQ2" s="111"/>
-      <c r="PR2" s="111"/>
-      <c r="PS2" s="112"/>
+      <c r="OT2" s="113"/>
+      <c r="OU2" s="113"/>
+      <c r="OV2" s="113"/>
+      <c r="OW2" s="113"/>
+      <c r="OX2" s="113"/>
+      <c r="OY2" s="113"/>
+      <c r="OZ2" s="113"/>
+      <c r="PA2" s="113"/>
+      <c r="PB2" s="113"/>
+      <c r="PC2" s="113"/>
+      <c r="PD2" s="113"/>
+      <c r="PE2" s="113"/>
+      <c r="PF2" s="113"/>
+      <c r="PG2" s="113"/>
+      <c r="PH2" s="113"/>
+      <c r="PI2" s="113"/>
+      <c r="PJ2" s="113"/>
+      <c r="PK2" s="113"/>
+      <c r="PL2" s="113"/>
+      <c r="PM2" s="113"/>
+      <c r="PN2" s="113"/>
+      <c r="PO2" s="113"/>
+      <c r="PP2" s="113"/>
+      <c r="PQ2" s="113"/>
+      <c r="PR2" s="113"/>
+      <c r="PS2" s="114"/>
     </row>
     <row r="3" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="85"/>
@@ -5021,7 +5036,7 @@
       <c r="PS5" s="90"/>
     </row>
     <row r="6" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="114"/>
+      <c r="B6" s="111"/>
       <c r="C6" s="97">
         <v>0</v>
       </c>
@@ -5459,7 +5474,7 @@
       <c r="PS6" s="95"/>
     </row>
     <row r="7" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="113" t="str">
+      <c r="B7" s="110" t="str">
         <f>Donnees!$C$22</f>
         <v>Mise en place Trello</v>
       </c>
@@ -5900,7 +5915,7 @@
       <c r="PS7" s="90"/>
     </row>
     <row r="8" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="114"/>
+      <c r="B8" s="111"/>
       <c r="C8" s="97">
         <v>0</v>
       </c>
@@ -6338,7 +6353,7 @@
       <c r="PS8" s="95"/>
     </row>
     <row r="9" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="113" t="str">
+      <c r="B9" s="110" t="str">
         <f>Donnees!$C$23</f>
         <v>Mise en place GitKraken</v>
       </c>
@@ -6779,7 +6794,7 @@
       <c r="PS9" s="90"/>
     </row>
     <row r="10" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="114"/>
+      <c r="B10" s="111"/>
       <c r="C10" s="97">
         <v>0</v>
       </c>
@@ -7217,7 +7232,7 @@
       <c r="PS10" s="95"/>
     </row>
     <row r="11" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="113" t="str">
+      <c r="B11" s="110" t="str">
         <f>Donnees!$C$24</f>
         <v>Mise à jour Trello</v>
       </c>
@@ -7658,7 +7673,7 @@
       <c r="PS11" s="90"/>
     </row>
     <row r="12" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="114"/>
+      <c r="B12" s="111"/>
       <c r="C12" s="97">
         <v>0</v>
       </c>
@@ -8096,7 +8111,7 @@
       <c r="PS12" s="95"/>
     </row>
     <row r="13" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="113" t="str">
+      <c r="B13" s="110" t="str">
         <f>Donnees!$C$25</f>
         <v>Mise à jour GitKraken</v>
       </c>
@@ -8537,7 +8552,7 @@
       <c r="PS13" s="90"/>
     </row>
     <row r="14" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="114"/>
+      <c r="B14" s="111"/>
       <c r="C14" s="97">
         <v>0</v>
       </c>
@@ -8975,7 +8990,7 @@
       <c r="PS14" s="95"/>
     </row>
     <row r="15" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="113" t="str">
+      <c r="B15" s="110" t="str">
         <f>Donnees!$C$26</f>
         <v>Recherches</v>
       </c>
@@ -9417,7 +9432,7 @@
     </row>
     <row r="16" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="104"/>
-      <c r="B16" s="114"/>
+      <c r="B16" s="111"/>
       <c r="C16" s="97">
         <v>0</v>
       </c>
@@ -9855,7 +9870,7 @@
       <c r="PS16" s="95"/>
     </row>
     <row r="17" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="113" t="str">
+      <c r="B17" s="110" t="str">
         <f>Donnees!$C$27</f>
         <v>Création plannif + JDT</v>
       </c>
@@ -10296,7 +10311,7 @@
       <c r="PS17" s="90"/>
     </row>
     <row r="18" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="114"/>
+      <c r="B18" s="111"/>
       <c r="C18" s="97">
         <v>0</v>
       </c>
@@ -10734,7 +10749,7 @@
       <c r="PS18" s="95"/>
     </row>
     <row r="19" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="113" t="str">
+      <c r="B19" s="110" t="str">
         <f>Donnees!$C$28</f>
         <v>Mise à jour du JDT</v>
       </c>
@@ -11175,7 +11190,7 @@
       <c r="PS19" s="90"/>
     </row>
     <row r="20" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="114"/>
+      <c r="B20" s="111"/>
       <c r="C20" s="97">
         <v>0</v>
       </c>
@@ -11613,7 +11628,7 @@
       <c r="PS20" s="95"/>
     </row>
     <row r="21" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="113" t="str">
+      <c r="B21" s="110" t="str">
         <f>Donnees!$C$29</f>
         <v>Daily Scrum</v>
       </c>
@@ -12054,7 +12069,7 @@
       <c r="PS21" s="90"/>
     </row>
     <row r="22" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="114"/>
+      <c r="B22" s="111"/>
       <c r="C22" s="97">
         <v>0</v>
       </c>
@@ -12492,7 +12507,7 @@
       <c r="PS22" s="95"/>
     </row>
     <row r="23" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="113" t="str">
+      <c r="B23" s="110" t="str">
         <f>Donnees!$C$30</f>
         <v>HTML</v>
       </c>
@@ -12933,7 +12948,7 @@
       <c r="PS23" s="90"/>
     </row>
     <row r="24" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="114"/>
+      <c r="B24" s="111"/>
       <c r="C24" s="97">
         <v>0</v>
       </c>
@@ -13371,7 +13386,7 @@
       <c r="PS24" s="95"/>
     </row>
     <row r="25" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="113" t="str">
+      <c r="B25" s="110" t="str">
         <f>Donnees!$C$31</f>
         <v>Base de donnée</v>
       </c>
@@ -13812,7 +13827,7 @@
       <c r="PS25" s="90"/>
     </row>
     <row r="26" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="114"/>
+      <c r="B26" s="111"/>
       <c r="C26" s="97">
         <v>0</v>
       </c>
@@ -14250,7 +14265,7 @@
       <c r="PS26" s="95"/>
     </row>
     <row r="27" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="113" t="str">
+      <c r="B27" s="110" t="str">
         <f>Donnees!$C$32</f>
         <v>PHP</v>
       </c>
@@ -14691,7 +14706,7 @@
       <c r="PS27" s="90"/>
     </row>
     <row r="28" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="114"/>
+      <c r="B28" s="111"/>
       <c r="C28" s="97">
         <v>0</v>
       </c>
@@ -15129,7 +15144,7 @@
       <c r="PS28" s="95"/>
     </row>
     <row r="29" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="113" t="str">
+      <c r="B29" s="110" t="str">
         <f>Donnees!$C$33</f>
         <v>Typo3</v>
       </c>
@@ -15570,7 +15585,7 @@
       <c r="PS29" s="90"/>
     </row>
     <row r="30" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="114"/>
+      <c r="B30" s="111"/>
       <c r="C30" s="97">
         <v>0</v>
       </c>
@@ -16008,7 +16023,7 @@
       <c r="PS30" s="95"/>
     </row>
     <row r="31" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="113" t="str">
+      <c r="B31" s="110" t="str">
         <f>Donnees!$C$34</f>
         <v>Création jeu flash</v>
       </c>
@@ -16449,7 +16464,7 @@
       <c r="PS31" s="90"/>
     </row>
     <row r="32" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="114"/>
+      <c r="B32" s="111"/>
       <c r="C32" s="97">
         <v>0</v>
       </c>
@@ -17771,14 +17786,13 @@
   </sheetData>
   <sheetProtection insertRows="0" selectLockedCells="1"/>
   <mergeCells count="31">
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="HL2:IL2"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="CG2:DG2"/>
-    <mergeCell ref="DH2:EH2"/>
-    <mergeCell ref="EI2:FI2"/>
-    <mergeCell ref="FJ2:GJ2"/>
-    <mergeCell ref="GK2:HK2"/>
+    <mergeCell ref="OS2:PS2"/>
+    <mergeCell ref="IM2:JM2"/>
+    <mergeCell ref="JN2:KN2"/>
+    <mergeCell ref="KO2:LO2"/>
+    <mergeCell ref="LP2:MP2"/>
+    <mergeCell ref="MQ2:NQ2"/>
+    <mergeCell ref="NR2:OR2"/>
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="D2:AD2"/>
@@ -17795,13 +17809,14 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
-    <mergeCell ref="OS2:PS2"/>
-    <mergeCell ref="IM2:JM2"/>
-    <mergeCell ref="JN2:KN2"/>
-    <mergeCell ref="KO2:LO2"/>
-    <mergeCell ref="LP2:MP2"/>
-    <mergeCell ref="MQ2:NQ2"/>
-    <mergeCell ref="NR2:OR2"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="HL2:IL2"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="CG2:DG2"/>
+    <mergeCell ref="DH2:EH2"/>
+    <mergeCell ref="EI2:FI2"/>
+    <mergeCell ref="FJ2:GJ2"/>
+    <mergeCell ref="GK2:HK2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="DureeTropLongue" error="Cette durée est invalide: ce n'est pas un chiffre entier positif ou elle dépasse la &quot;Durée totale&quot; définie plus haut ..." sqref="C33">
@@ -20472,8 +20487,8 @@
   </sheetPr>
   <dimension ref="A1:I293"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20832,39 +20847,75 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="13"/>
+      <c r="A29" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="8">
+        <v>1</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>66</v>
+      </c>
       <c r="D29" s="13"/>
     </row>
     <row r="30" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="14"/>
+      <c r="A30" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="6">
+        <v>5</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>67</v>
+      </c>
       <c r="D30" s="14"/>
     </row>
-    <row r="31" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="14"/>
+    <row r="31" spans="1:9" ht="216" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="6">
+        <v>13</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>68</v>
+      </c>
       <c r="D31" s="14"/>
     </row>
-    <row r="32" spans="1:9" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="14"/>
+    <row r="32" spans="1:9" ht="27" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="6">
+        <v>5</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>70</v>
+      </c>
       <c r="D32" s="14"/>
     </row>
     <row r="33" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="5"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="14"/>
+      <c r="A33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="6">
+        <v>2</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>69</v>
+      </c>
       <c r="D33" s="14"/>
     </row>
     <row r="34" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="14"/>
+      <c r="A34" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="6">
+        <v>1</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>63</v>
+      </c>
       <c r="D34" s="14"/>
     </row>
     <row r="35" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
@@ -20927,7 +20978,7 @@
       </c>
       <c r="B44" s="76">
         <f>SUM(B29:B43)</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C44" s="107" t="s">
         <v>44</v>

</xml_diff>